<commit_message>
fix: generate real number
</commit_message>
<xml_diff>
--- a/templates.xlsx
+++ b/templates.xlsx
@@ -302,7 +302,7 @@
     <t>这一年手术量排名前几的科室编码和名称？</t>
   </si>
   <si>
-    <t>在（时间段）内手术量排名前（几）的科室编码和名称？</t>
+    <t>在（时间段）内手术量排名前（整数）的科室编码和名称？</t>
   </si>
   <si>
     <t>SELECT MED_ORG_DEPT_CD, MED_ORG_DEPT_NM FROM t_kc22 WHERE STA_DATE BETWEEN $1 AND $2 AND MED_INV_ITEM_TYPE = 24 GROUP BY MED_ORG_DEPT_CD ORDER BY COUNT(*) DESC LIMIT $3</t>
@@ -311,7 +311,7 @@
     <t>这一年手术量排名倒数的科室编码和名称？</t>
   </si>
   <si>
-    <t>在（时间段）内手术量排名倒数前（几）的科室编码和名称？</t>
+    <t>在（时间段）内手术量排名倒数前（整数）的科室编码和名称？</t>
   </si>
   <si>
     <t>SELECT MED_ORG_DEPT_CD, MED_ORG_DEPT_NM FROM t_kc22 WHERE STA_DATE BETWEEN $1 AND $2 AND MED_INV_ITEM_TYPE = 24 GROUP BY MED_ORG_DEPT_CD ORDER BY COUNT(*) ASC LIMIT $3</t>
@@ -338,7 +338,7 @@
     <t>某医院年度统筹金额哪些科室消耗得多？</t>
   </si>
   <si>
-    <t>医疗机构（医疗机构代码）在（时间段）内统筹金额消耗最多的（几）个科室是哪些？</t>
+    <t>医疗机构（医疗机构代码）在（时间段）内统筹金额消耗最多的（整数）个科室是哪些？</t>
   </si>
   <si>
     <t>SELECT t_kc21.MED_ORG_DEPT_CD, t_kc21.MED_ORG_DEPT_NM FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 AND t_kc24.CLINIC_SLT_DATE BETWEEN $2 AND $3 GROUP BY t_kc21.MED_ORG_DEPT_CD ORDER BY SUM(t_kc24.OVE_PAY) DESC LIMIT $4</t>
@@ -410,7 +410,7 @@
     <t>某医院住院天数&gt;180天的人数？</t>
   </si>
   <si>
-    <t>医疗机构（医疗机构代码）住院天数超过（几）天的人数？</t>
+    <t>医疗机构（医疗机构代码）住院天数超过（整数）天的人数？</t>
   </si>
   <si>
     <t>SELECT COUNT(DISTINCT hz_info.RYBH) FROM hz_info JOIN zyjzjlb ON hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX WHERE zyjzjlb.YLJGDM = $1 AND CYSJ - RYSJ &gt; $2</t>
@@ -563,7 +563,7 @@
     <t>某医院使用次数top10的项目？</t>
   </si>
   <si>
-    <t>医疗机构（医疗机构代码）使用次数top（几）的项目？</t>
+    <t>医疗机构（医疗机构代码）使用次数top（整数）的项目？</t>
   </si>
   <si>
     <t>SELECT t_kc22.SOC_SRT_DIRE_CD, t_kc22.SOC_SRT_DIRE_NM FROM t_kc21 JOIN t_kc22 ON t_kc21.MED_CLINIC_ID = t_kc22.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 GROUP BY t_kc22.SOC_SRT_DIRE_CD ORDER BY COUNT(*) DESC LIMIT $2</t>
@@ -572,7 +572,7 @@
     <t>某医院金额top10的项目？</t>
   </si>
   <si>
-    <t>医疗机构（医疗机构代码）金额top（几）的项目？</t>
+    <t>医疗机构（医疗机构代码）金额top（整数）的项目？</t>
   </si>
   <si>
     <t>SELECT t_kc22.SOC_SRT_DIRE_CD, t_kc22.SOC_SRT_DIRE_NM FROM t_kc21 JOIN t_kc22 ON t_kc21.MED_CLINIC_ID = t_kc22.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 GROUP BY t_kc22.SOC_SRT_DIRE_CD ORDER BY SUM(t_kc22.AMOUNT) DESC LIMIT $2</t>
@@ -1193,7 +1193,7 @@
     <t>某医疗机构一年内未就业人员医疗就诊的医疗费总额达到10000元以上的就诊记录数量</t>
   </si>
   <si>
-    <t>医疗机构（医疗机构代码）在（时间段）内未就业人员医疗就诊的医疗费总额达到（几）元以上的就诊记录数量</t>
+    <t>医疗机构（医疗机构代码）在（时间段）内未就业人员医疗就诊的医疗费总额达到（大实数）元以上的就诊记录数量</t>
   </si>
   <si>
     <t>SELECT COUNT(*) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 AND IN_HOSP_DATE BETWEEN $2 AND $3 AND INSURED_STS = 0 AND MED_AMOUT &gt;= $4</t>
@@ -1343,13 +1343,13 @@
     <t>某患者一年内自付比例低于50%的药品量</t>
   </si>
   <si>
-    <t>患者（人员ID）在（时间段）内自付比例低于（几）的药品量</t>
+    <t>患者（人员ID）在（时间段）内自付比例低于（小实数）的药品量</t>
   </si>
   <si>
     <t>SELECT COUNT(*) FROM t_kc21 JOIN t_kc22 ON t_kc21.MED_CLINIC_ID = t_kc22.MED_CLINIC_ID WHERE t_kc21.PERSON_ID = $1 AND t_kc22.STA_DATE BETWEEN $2 AND $3 AND t_kc22.SELF_PAY_PRO &lt; $4</t>
   </si>
   <si>
-    <t>患者（人员姓名）在（时间段）内自付比例低于（几）的药品量</t>
+    <t>患者（人员姓名）在（时间段）内自付比例低于（小实数）的药品量</t>
   </si>
   <si>
     <t>SELECT COUNT(*) FROM t_kc21 JOIN t_kc22 ON t_kc21.MED_CLINIC_ID = t_kc22.MED_CLINIC_ID WHERE t_kc21.PERSON_NM = $1 AND t_kc22.STA_DATE BETWEEN $2 AND $3 AND t_kc22.SELF_PAY_PRO &lt; $4</t>
@@ -1358,13 +1358,13 @@
     <t>某患者一年内自费金额高于1000元的药品量</t>
   </si>
   <si>
-    <t>患者（人员ID）在（时间段）内自费金额高于（几）元的药品量</t>
+    <t>患者（人员ID）在（时间段）内自费金额高于（大实数）元的药品量</t>
   </si>
   <si>
     <t>SELECT COUNT(*) FROM t_kc21 JOIN t_kc22 ON t_kc21.MED_CLINIC_ID = t_kc22.MED_CLINIC_ID WHERE t_kc21.PERSON_ID = $1 AND t_kc22.STA_DATE BETWEEN $2 AND $3 AND t_kc22.SELF_PAY_AMO &gt; $4</t>
   </si>
   <si>
-    <t>患者（人员姓名）在（时间段）内自费金额高于（几）元的药品量</t>
+    <t>患者（人员姓名）在（时间段）内自费金额高于（大实数）元的药品量</t>
   </si>
   <si>
     <t>SELECT COUNT(*) FROM t_kc21 JOIN t_kc22 ON t_kc21.MED_CLINIC_ID = t_kc22.MED_CLINIC_ID WHERE t_kc21.PERSON_NM = $1 AND t_kc22.STA_DATE BETWEEN $2 AND $3 AND t_kc22.SELF_PAY_AMO &gt; $4</t>
@@ -1373,7 +1373,7 @@
     <t>列出某次医疗就诊开出药品的定价上限金额高于1000元的所有药品</t>
   </si>
   <si>
-    <t>列出医疗就诊（医疗就诊ID）中开出药品的定价上限金额高于（几）元的所有药品</t>
+    <t>列出医疗就诊（医疗就诊ID）中开出药品的定价上限金额高于（大实数）元的所有药品</t>
   </si>
   <si>
     <t>SELECT SOC_SRT_DIRE_CD, SOC_SRT_DIRE_NM FROM t_kc22 WHERE MED_CLINIC_ID = $1 AND UP_LIMIT_AMO &gt; $2</t>
@@ -1382,7 +1382,7 @@
     <t>列出某次医疗就诊开出药品的超限价自付金额高于100元的所有药品</t>
   </si>
   <si>
-    <t>列出医疗就诊（医疗就诊ID）中开出药品的超限价自付金额高于（几）元的所有药品</t>
+    <t>列出医疗就诊（医疗就诊ID）中开出药品的超限价自付金额高于（大实数）元的所有药品</t>
   </si>
   <si>
     <t>SELECT SOC_SRT_DIRE_CD, SOC_SRT_DIRE_NM FROM t_kc22 WHERE MED_CLINIC_ID = $1 AND OVE_SELF_AMO &gt; $2</t>
@@ -1778,7 +1778,7 @@
     <t>某医疗机构某个月中住院时长超过一周的住院就诊记录数</t>
   </si>
   <si>
-    <t>医疗机构（医疗机构代码）在（时间段）内住院时长超过（几）天的住院就诊记录数</t>
+    <t>医疗机构（医疗机构代码）在（时间段）内住院时长超过（整数）天的住院就诊记录数</t>
   </si>
   <si>
     <t>SELECT COUNT(*) FROM zyjzjlb WHERE YLJGDM = $1 AND RYDJSJ BETWEEN $2 AND $3 AND CYSJ - RYSJ &gt; $4</t>
@@ -2225,25 +2225,25 @@
     <t>把某市开药天数&gt;500天的患者按就诊医生聚集列出来</t>
   </si>
   <si>
-    <t>把（地点）开药时长超过（几）天的患者按就诊医生聚集列出来</t>
+    <t>把（地点）开药时长超过（整数）天的患者按就诊医生聚集列出来</t>
   </si>
   <si>
     <t>把某市开药天数&gt;500天的患者按就诊医院聚集列出来</t>
   </si>
   <si>
-    <t>把（地点）开药时长超过（几）天的患者按就诊医院聚集列出来</t>
+    <t>把（地点）开药时长超过（整数）天的患者按就诊医院聚集列出来</t>
   </si>
   <si>
     <t>把某市全年在一个小时（天/5分钟）内共同就诊的参保人对列出来</t>
   </si>
   <si>
-    <t>把（地点）在（时间段）内在（几）天内共同就诊的参保人对列出来</t>
+    <t>把（地点）在（时间段）内在（整数）天内共同就诊的参保人对列出来</t>
   </si>
   <si>
     <t>把某市全年开药次数&gt;50（100/200）的参保人及其开药次数列出来</t>
   </si>
   <si>
-    <t>把（地点）在（时间段）内开药次数超过（几）次的参保人及其开药次数列出来</t>
+    <t>把（地点）在（时间段）内开药次数超过（整数）次的参保人及其开药次数列出来</t>
   </si>
   <si>
     <t>某参保人年度小金额结算次数，10元以内为小金额</t>
@@ -2488,7 +2488,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:xvml="urn:schemas-microsoft-com:office:excel" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:pvml="urn:schemas-microsoft-com:office:powerpoint" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:odx="http://opendope.org/xpaths" xmlns:odc="http://opendope.org/conditions" xmlns:odq="http://opendope.org/questions" xmlns:oda="http://opendope.org/answers" xmlns:odi="http://opendope.org/components" xmlns:odgm="http://opendope.org/SmartArt/DataHierarchy" xmlns:b="http://schemas.openxmlformats.org/officeDocument/2006/bibliography" xmlns:w16se="http://schemas.microsoft.com/office/word/2015/wordml/symex" xmlns:w16cid="http://schemas.microsoft.com/office/word/2016/wordml/cid" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" name="">
+<a:theme xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:xvml="urn:schemas-microsoft-com:office:excel" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:pvml="urn:schemas-microsoft-com:office:powerpoint" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:odx="http://opendope.org/xpaths" xmlns:odc="http://opendope.org/conditions" xmlns:odq="http://opendope.org/questions" xmlns:oda="http://opendope.org/answers" xmlns:odi="http://opendope.org/components" xmlns:odgm="http://opendope.org/SmartArt/DataHierarchy" xmlns:b="http://schemas.openxmlformats.org/officeDocument/2006/bibliography" xmlns:w16se="http://schemas.microsoft.com/office/word/2015/wordml/symex" xmlns:w16cid="http://schemas.microsoft.com/office/word/2016/wordml/cid" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" name="">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>

</xml_diff>

<commit_message>
feat: schema for yiliao
</commit_message>
<xml_diff>
--- a/templates.xlsx
+++ b/templates.xlsx
@@ -413,7 +413,7 @@
     <t>医疗机构（医疗机构代码）住院天数超过（整数）天的人数？</t>
   </si>
   <si>
-    <t>SELECT COUNT(DISTINCT hz_info.RYBH) FROM hz_info JOIN zyjzjlb ON hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX WHERE zyjzjlb.YLJGDM = $1 AND CYSJ - RYSJ &gt; $2</t>
+    <t>SELECT COUNT(DISTINCT hz_info.RYBH) FROM hz_info JOIN zyjzjlb ON hz_info.YLJGDM = zyjzjlb.YLJGDM AND hz_info.KH = zyjzjlb.KH AND hz_info.KLX = zyjzjlb.KLX WHERE zyjzjlb.YLJGDM = $1 AND DATEDIFF(zyjzjlb.CYSJ, zyjzjlb.RYSJ) &gt; $2</t>
   </si>
   <si>
     <t>某医院异地就医人数？</t>
@@ -788,13 +788,13 @@
     <t>患者（人员ID）在（时间段）内在医疗机构（医疗机构代码）的门诊就诊次数</t>
   </si>
   <si>
-    <t>SELECT COUNT(*) FROM hz_info JOIN mzjzjlb ON hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX WHERE hz_info.RYBH = $1 AND JZKSRQ BETWEEN $2 AND $3 AND mzjzjlb.YLJGDM = $4</t>
+    <t>SELECT COUNT(*) FROM hz_info JOIN mzjzjlb ON hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX WHERE hz_info.RYBH = $1 AND mzjzjlb.JZKSRQ BETWEEN $2 AND $3 AND mzjzjlb.YLJGDM = $4</t>
   </si>
   <si>
     <t>患者（人员姓名）在（时间段）内在医疗机构（医疗机构代码）的门诊就诊次数</t>
   </si>
   <si>
-    <t>SELECT COUNT(*) FROM person_info JOIN hz_info JOIN mzjzjlb ON person_info.RYBH = hz_info.RYBH AND hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX WHERE person_info.XM = $1 AND JZKSRQ BETWEEN $2 AND $3 AND mzjzjlb.YLJGDM = $4</t>
+    <t>SELECT COUNT(*) FROM person_info JOIN hz_info JOIN mzjzjlb ON person_info.RYBH = hz_info.RYBH AND hz_info.YLJGDM = mzjzjlb.YLJGDM AND hz_info.KH = mzjzjlb.KH AND hz_info.KLX = mzjzjlb.KLX WHERE person_info.XM = $1 AND mzjzjlb.JZKSRQ BETWEEN $2 AND $3 AND mzjzjlb.YLJGDM = $4</t>
   </si>
   <si>
     <t>某医疗机构某月处理的新生儿门诊就诊次数</t>
@@ -1781,7 +1781,7 @@
     <t>医疗机构（医疗机构代码）在（时间段）内住院时长超过（整数）天的住院就诊记录数</t>
   </si>
   <si>
-    <t>SELECT COUNT(*) FROM zyjzjlb WHERE YLJGDM = $1 AND RYDJSJ BETWEEN $2 AND $3 AND CYSJ - RYSJ &gt; $4</t>
+    <t>SELECT COUNT(*) FROM zyjzjlb WHERE YLJGDM = $1 AND RYDJSJ BETWEEN $2 AND $3 AND DATEDIFF(CYSJ, RYSJ) &gt; $4</t>
   </si>
   <si>
     <t>某次住院就诊的出院状态代码</t>
@@ -2488,7 +2488,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:xvml="urn:schemas-microsoft-com:office:excel" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:pvml="urn:schemas-microsoft-com:office:powerpoint" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:odx="http://opendope.org/xpaths" xmlns:odc="http://opendope.org/conditions" xmlns:odq="http://opendope.org/questions" xmlns:oda="http://opendope.org/answers" xmlns:odi="http://opendope.org/components" xmlns:odgm="http://opendope.org/SmartArt/DataHierarchy" xmlns:b="http://schemas.openxmlformats.org/officeDocument/2006/bibliography" xmlns:w16se="http://schemas.microsoft.com/office/word/2015/wordml/symex" xmlns:w16cid="http://schemas.microsoft.com/office/word/2016/wordml/cid" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" name="">
+<a:theme xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:xvml="urn:schemas-microsoft-com:office:excel" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:pvml="urn:schemas-microsoft-com:office:powerpoint" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:odx="http://opendope.org/xpaths" xmlns:odc="http://opendope.org/conditions" xmlns:odq="http://opendope.org/questions" xmlns:oda="http://opendope.org/answers" xmlns:odi="http://opendope.org/components" xmlns:odgm="http://opendope.org/SmartArt/DataHierarchy" xmlns:b="http://schemas.openxmlformats.org/officeDocument/2006/bibliography" xmlns:w16se="http://schemas.microsoft.com/office/word/2015/wordml/symex" xmlns:w16cid="http://schemas.microsoft.com/office/word/2016/wordml/cid" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" name="">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>

</xml_diff>